<commit_message>
Facitliste til musik tjekket.
</commit_message>
<xml_diff>
--- a/undervisningsforlob/musik/musik.xlsx
+++ b/undervisningsforlob/musik/musik.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruger\Documents\GitHub\aalborg-intelligence.github.io\undervisningsforlob\musik\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C019B0E8-2C38-4BB9-9A15-8C219398E352}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6E738E1-AF7E-4923-9CB6-2BC2A760599B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10370" yWindow="540" windowWidth="16370" windowHeight="13410" xr2:uid="{87057390-18A9-4D94-9772-89AC3B7E8D79}"/>
+    <workbookView xWindow="15550" yWindow="430" windowWidth="16400" windowHeight="13250" xr2:uid="{87057390-18A9-4D94-9772-89AC3B7E8D79}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Nummer</t>
   </si>
@@ -93,108 +93,6 @@
   </si>
   <si>
     <t>White Iverson</t>
-  </si>
-  <si>
-    <t>0.76</t>
-  </si>
-  <si>
-    <t>0.83</t>
-  </si>
-  <si>
-    <t>0.60</t>
-  </si>
-  <si>
-    <t>0.53</t>
-  </si>
-  <si>
-    <t>0.64</t>
-  </si>
-  <si>
-    <t>0.78</t>
-  </si>
-  <si>
-    <t>0.90</t>
-  </si>
-  <si>
-    <t>0.51</t>
-  </si>
-  <si>
-    <t>0.82</t>
-  </si>
-  <si>
-    <t>0.42</t>
-  </si>
-  <si>
-    <t>0.67</t>
-  </si>
-  <si>
-    <t>0.95</t>
-  </si>
-  <si>
-    <t>0.65</t>
-  </si>
-  <si>
-    <t>0.70</t>
-  </si>
-  <si>
-    <t>0.84</t>
-  </si>
-  <si>
-    <t>0.72</t>
-  </si>
-  <si>
-    <t>0.74</t>
-  </si>
-  <si>
-    <t>0.71</t>
-  </si>
-  <si>
-    <t>0.80</t>
-  </si>
-  <si>
-    <t>0.59</t>
-  </si>
-  <si>
-    <t>0.62</t>
-  </si>
-  <si>
-    <t>0.97</t>
-  </si>
-  <si>
-    <t>0.52</t>
-  </si>
-  <si>
-    <t>0.04</t>
-  </si>
-  <si>
-    <t>0.08</t>
-  </si>
-  <si>
-    <t>0.05</t>
-  </si>
-  <si>
-    <t>0.09</t>
-  </si>
-  <si>
-    <t>0.02</t>
-  </si>
-  <si>
-    <t>0.03</t>
-  </si>
-  <si>
-    <t>0.07</t>
-  </si>
-  <si>
-    <t>0.21</t>
-  </si>
-  <si>
-    <t>0.37</t>
-  </si>
-  <si>
-    <t>0.06</t>
-  </si>
-  <si>
-    <t>0.14</t>
   </si>
 </sst>
 </file>
@@ -601,210 +499,210 @@
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>42</v>
+      <c r="B2" s="1">
+        <v>0.76</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0.04</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>43</v>
+      <c r="B3" s="1">
+        <v>0.83</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.65</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.08</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>46</v>
+      <c r="B4" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.67</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.02</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>44</v>
+      <c r="B5" s="1">
+        <v>0.53</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.78</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.05</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>47</v>
+      <c r="B6" s="1">
+        <v>0.76</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.03</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>42</v>
+      <c r="B7" s="1">
+        <v>0.64</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.84</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.04</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>48</v>
+      <c r="B8" s="1">
+        <v>0.76</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0.72</v>
+      </c>
+      <c r="D8" s="1">
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>49</v>
+      <c r="B9" s="1">
+        <v>0.78</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0.74</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0.21</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>50</v>
+      <c r="B10" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0.71</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0.37</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>51</v>
+      <c r="B11" s="1">
+        <v>0.51</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0.06</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>44</v>
+      <c r="B12" s="1">
+        <v>0.76</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0.05</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>45</v>
+      <c r="B13" s="1">
+        <v>0.82</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0.59</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0.09</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>51</v>
+      <c r="B14" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0.62</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0.06</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>52</v>
+      <c r="B15" s="1">
+        <v>0.42</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0.97</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>42</v>
+      <c r="B16" s="1">
+        <v>0.67</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0.52</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0.04</v>
       </c>
     </row>
   </sheetData>

</xml_diff>